<commit_message>
Separação das funções do programa principal
</commit_message>
<xml_diff>
--- a/dash/PLANILHA TAF.xlsx
+++ b/dash/PLANILHA TAF.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1º TAF" sheetId="1" r:id="rId1"/>
@@ -900,10 +900,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A41" sqref="A41:N42"/>
     </sheetView>
@@ -987,7 +986,7 @@
       <c r="AC1" s="5"/>
       <c r="AD1" s="6"/>
     </row>
-    <row r="2" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="2" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
@@ -1045,7 +1044,7 @@
       <c r="AC2" s="8"/>
       <c r="AD2" s="10"/>
     </row>
-    <row r="3" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="3" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
@@ -1103,7 +1102,7 @@
       <c r="AC3" s="8"/>
       <c r="AD3" s="10"/>
     </row>
-    <row r="4" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="4" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -1161,7 +1160,7 @@
       <c r="AC4" s="8"/>
       <c r="AD4" s="10"/>
     </row>
-    <row r="5" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="5" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
@@ -1277,7 +1276,7 @@
       <c r="AC6" s="8"/>
       <c r="AD6" s="10"/>
     </row>
-    <row r="7" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="7" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A7" s="7" t="s">
         <v>47</v>
       </c>
@@ -1335,7 +1334,7 @@
       <c r="AC7" s="8"/>
       <c r="AD7" s="10"/>
     </row>
-    <row r="8" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="8" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A8" s="7" t="s">
         <v>47</v>
       </c>
@@ -1393,7 +1392,7 @@
       <c r="AC8" s="8"/>
       <c r="AD8" s="10"/>
     </row>
-    <row r="9" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="9" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
@@ -1451,7 +1450,7 @@
       <c r="AC9" s="8"/>
       <c r="AD9" s="10"/>
     </row>
-    <row r="10" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A10" s="7" t="s">
         <v>50</v>
       </c>
@@ -1509,7 +1508,7 @@
       <c r="AC10" s="8"/>
       <c r="AD10" s="10"/>
     </row>
-    <row r="11" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="11" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A11" s="7" t="s">
         <v>50</v>
       </c>
@@ -1683,7 +1682,7 @@
       <c r="AC13" s="8"/>
       <c r="AD13" s="10"/>
     </row>
-    <row r="14" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="14" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A14" s="7" t="s">
         <v>41</v>
       </c>
@@ -1741,7 +1740,7 @@
       <c r="AC14" s="8"/>
       <c r="AD14" s="10"/>
     </row>
-    <row r="15" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="15" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
@@ -1799,7 +1798,7 @@
       <c r="AC15" s="8"/>
       <c r="AD15" s="10"/>
     </row>
-    <row r="16" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="16" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A16" s="7" t="s">
         <v>41</v>
       </c>
@@ -1857,7 +1856,7 @@
       <c r="AC16" s="8"/>
       <c r="AD16" s="10"/>
     </row>
-    <row r="17" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="17" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A17" s="7" t="s">
         <v>46</v>
       </c>
@@ -1915,7 +1914,7 @@
       <c r="AC17" s="8"/>
       <c r="AD17" s="10"/>
     </row>
-    <row r="18" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A18" s="7" t="s">
         <v>46</v>
       </c>
@@ -1969,7 +1968,7 @@
       <c r="AC18" s="8"/>
       <c r="AD18" s="10"/>
     </row>
-    <row r="19" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="19" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -2027,7 +2026,7 @@
       <c r="AC19" s="8"/>
       <c r="AD19" s="10"/>
     </row>
-    <row r="20" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="20" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A20" s="7" t="s">
         <v>52</v>
       </c>
@@ -2083,7 +2082,7 @@
       <c r="AC20" s="8"/>
       <c r="AD20" s="10"/>
     </row>
-    <row r="21" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="21" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A21" s="7" t="s">
         <v>97</v>
       </c>
@@ -2141,7 +2140,7 @@
       <c r="AC21" s="8"/>
       <c r="AD21" s="10"/>
     </row>
-    <row r="22" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="22" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A22" s="7" t="s">
         <v>52</v>
       </c>
@@ -2201,7 +2200,7 @@
       <c r="AC22" s="8"/>
       <c r="AD22" s="10"/>
     </row>
-    <row r="23" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="23" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A23" s="7" t="s">
         <v>52</v>
       </c>
@@ -2259,7 +2258,7 @@
       <c r="AC23" s="8"/>
       <c r="AD23" s="10"/>
     </row>
-    <row r="24" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="24" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A24" s="7" t="s">
         <v>54</v>
       </c>
@@ -2317,7 +2316,7 @@
       <c r="AC24" s="8"/>
       <c r="AD24" s="10"/>
     </row>
-    <row r="25" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="25" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A25" s="7" t="s">
         <v>38</v>
       </c>
@@ -2375,7 +2374,7 @@
       <c r="AC25" s="8"/>
       <c r="AD25" s="10"/>
     </row>
-    <row r="26" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="26" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A26" s="7" t="s">
         <v>38</v>
       </c>
@@ -2433,7 +2432,7 @@
       <c r="AC26" s="8"/>
       <c r="AD26" s="10"/>
     </row>
-    <row r="27" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="27" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A27" s="7" t="s">
         <v>38</v>
       </c>
@@ -2491,7 +2490,7 @@
       <c r="AC27" s="8"/>
       <c r="AD27" s="10"/>
     </row>
-    <row r="28" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="28" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A28" s="7" t="s">
         <v>39</v>
       </c>
@@ -2549,7 +2548,7 @@
       <c r="AC28" s="8"/>
       <c r="AD28" s="10"/>
     </row>
-    <row r="29" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="29" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A29" s="7" t="s">
         <v>39</v>
       </c>
@@ -2607,7 +2606,7 @@
       <c r="AC29" s="8"/>
       <c r="AD29" s="10"/>
     </row>
-    <row r="30" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="30" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A30" s="7" t="s">
         <v>39</v>
       </c>
@@ -2665,7 +2664,7 @@
       <c r="AC30" s="8"/>
       <c r="AD30" s="10"/>
     </row>
-    <row r="31" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="31" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A31" s="7" t="s">
         <v>39</v>
       </c>
@@ -2721,7 +2720,7 @@
       <c r="AC31" s="8"/>
       <c r="AD31" s="10"/>
     </row>
-    <row r="32" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="32" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A32" s="7" t="s">
         <v>39</v>
       </c>
@@ -2779,7 +2778,7 @@
       <c r="AC32" s="8"/>
       <c r="AD32" s="10"/>
     </row>
-    <row r="33" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="33" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A33" s="7" t="s">
         <v>40</v>
       </c>
@@ -2837,7 +2836,7 @@
       <c r="AC33" s="8"/>
       <c r="AD33" s="10"/>
     </row>
-    <row r="34" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="34" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A34" s="7" t="s">
         <v>40</v>
       </c>
@@ -2895,7 +2894,7 @@
       <c r="AC34" s="8"/>
       <c r="AD34" s="10"/>
     </row>
-    <row r="35" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="35" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A35" s="7" t="s">
         <v>40</v>
       </c>
@@ -2953,7 +2952,7 @@
       <c r="AC35" s="8"/>
       <c r="AD35" s="10"/>
     </row>
-    <row r="36" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="36" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A36" s="7" t="s">
         <v>40</v>
       </c>
@@ -3011,7 +3010,7 @@
       <c r="AC36" s="8"/>
       <c r="AD36" s="10"/>
     </row>
-    <row r="37" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="37" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A37" s="7" t="s">
         <v>40</v>
       </c>
@@ -3069,7 +3068,7 @@
       <c r="AC37" s="8"/>
       <c r="AD37" s="10"/>
     </row>
-    <row r="38" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="38" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>40</v>
       </c>
@@ -3125,7 +3124,7 @@
       <c r="AC38" s="8"/>
       <c r="AD38" s="10"/>
     </row>
-    <row r="39" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="39" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A39" s="7" t="s">
         <v>40</v>
       </c>
@@ -3173,7 +3172,7 @@
       <c r="AC39" s="8"/>
       <c r="AD39" s="10"/>
     </row>
-    <row r="40" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="40" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A40" s="7" t="s">
         <v>42</v>
       </c>
@@ -3521,7 +3520,7 @@
       <c r="AC45" s="8"/>
       <c r="AD45" s="10"/>
     </row>
-    <row r="46" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="46" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A46" s="7" t="s">
         <v>42</v>
       </c>
@@ -3633,7 +3632,7 @@
       <c r="AC47" s="8"/>
       <c r="AD47" s="10"/>
     </row>
-    <row r="48" spans="1:30" ht="13.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="48" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
       <c r="A48" s="7" t="s">
         <v>42</v>
       </c>
@@ -3809,11 +3808,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M50">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="2ª Cia Fuz L Mth"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A2:M1000">
       <sortCondition ref="A2:A1000" customList="CEL,TEN CEL,MAJ,CAP,1º TEN,2º TEN,ASP,S TEN,1º SGT,2º SGT,2º SGT QE,3º SGT,CB,SD,SD EV"/>
     </sortState>
@@ -3832,9 +3826,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14.25"/>

</xml_diff>